<commit_message>
Annotations from 3 annotators comb.
</commit_message>
<xml_diff>
--- a/annotation_guide_10pic/annotationguide_full.xlsx
+++ b/annotation_guide_10pic/annotationguide_full.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhm25\Desktop\ITU\github\Iguana_PIDS\annotation_guide_10pic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BF0F67F-8A85-4B90-886D-D52D211D1E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B0D355-CDB6-4F53-B10C-1BE470BBF249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FD719A5A-E84E-6643-A04D-464618061C8A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="151">
   <si>
     <t>Picture ID</t>
   </si>
@@ -483,19 +483,31 @@
   </si>
   <si>
     <t>PAT_996_6_622.png</t>
+  </si>
+  <si>
+    <t>mulitple lesions</t>
+  </si>
+  <si>
+    <t>multiple lesions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -518,8 +530,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -834,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B332D225-3110-8B45-A888-BE865E981B75}">
-  <dimension ref="A1:U129"/>
+  <dimension ref="A1:V129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -914,393 +928,2042 @@
       <c r="A2" t="s">
         <v>21</v>
       </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>4</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="O16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>3</v>
+      </c>
+      <c r="O17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>4</v>
+      </c>
+      <c r="O20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>3</v>
+      </c>
+      <c r="O21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>3</v>
+      </c>
+      <c r="O23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>2</v>
+      </c>
+      <c r="O24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>3</v>
+      </c>
+      <c r="O25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>4</v>
+      </c>
+      <c r="O26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2">
+        <v>1</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2">
+        <v>1</v>
+      </c>
+      <c r="P28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>2</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2">
+        <v>1</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2">
+        <v>2</v>
+      </c>
+      <c r="P29" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2">
+        <v>1</v>
+      </c>
+      <c r="J30" s="2">
+        <v>1</v>
+      </c>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2">
+        <v>2</v>
+      </c>
+      <c r="P30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>2</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2">
+        <v>3</v>
+      </c>
+      <c r="P31" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0</v>
+      </c>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2">
+        <v>2</v>
+      </c>
+      <c r="P32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1</v>
+      </c>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2">
+        <v>3</v>
+      </c>
+      <c r="P33" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2">
+        <v>0</v>
+      </c>
+      <c r="J34" s="2">
+        <v>1</v>
+      </c>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2">
+        <v>3</v>
+      </c>
+      <c r="P34" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <v>2</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1</v>
+      </c>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2">
+        <v>3</v>
+      </c>
+      <c r="P35" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2">
+        <v>1</v>
+      </c>
+      <c r="J36" s="2">
+        <v>0</v>
+      </c>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2">
+        <v>3</v>
+      </c>
+      <c r="P36" s="2">
+        <v>1</v>
+      </c>
+      <c r="V36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2">
+        <v>0</v>
+      </c>
+      <c r="J37" s="2">
+        <v>1</v>
+      </c>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2">
+        <v>3</v>
+      </c>
+      <c r="P37" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2">
+        <v>0</v>
+      </c>
+      <c r="J38" s="2">
+        <v>0</v>
+      </c>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2">
+        <v>2</v>
+      </c>
+      <c r="P38" s="2">
+        <v>1</v>
+      </c>
+      <c r="V38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" s="2">
+        <v>2</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2">
+        <v>1</v>
+      </c>
+      <c r="J39" s="2">
+        <v>1</v>
+      </c>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2">
+        <v>1</v>
+      </c>
+      <c r="P39" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2">
+        <v>0</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0</v>
+      </c>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2">
+        <v>3</v>
+      </c>
+      <c r="P40" s="2">
+        <v>1</v>
+      </c>
+      <c r="V40" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2">
+        <v>0</v>
+      </c>
+      <c r="J41" s="2">
+        <v>1</v>
+      </c>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2">
+        <v>4</v>
+      </c>
+      <c r="P41" s="2">
+        <v>3</v>
+      </c>
+      <c r="V41" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" s="2">
+        <v>2</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2">
+        <v>0</v>
+      </c>
+      <c r="J42" s="2">
+        <v>0</v>
+      </c>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2">
+        <v>2</v>
+      </c>
+      <c r="P42" s="2">
+        <v>2</v>
+      </c>
+      <c r="V42" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2">
+        <v>1</v>
+      </c>
+      <c r="J43" s="2">
+        <v>0</v>
+      </c>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2">
+        <v>1</v>
+      </c>
+      <c r="P43" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2">
+        <v>1</v>
+      </c>
+      <c r="J44" s="2">
+        <v>0</v>
+      </c>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2">
+        <v>2</v>
+      </c>
+      <c r="P44" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45" s="2">
+        <v>1</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2">
+        <v>1</v>
+      </c>
+      <c r="J45" s="2">
+        <v>0</v>
+      </c>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2">
+        <v>2</v>
+      </c>
+      <c r="P45" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2">
+        <v>2</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2">
+        <v>0</v>
+      </c>
+      <c r="J46" s="2">
+        <v>1</v>
+      </c>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2">
+        <v>2</v>
+      </c>
+      <c r="P46" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2">
+        <v>1</v>
+      </c>
+      <c r="J47" s="2">
+        <v>0</v>
+      </c>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2">
+        <v>1</v>
+      </c>
+      <c r="P47" s="2">
+        <v>2</v>
+      </c>
+      <c r="V47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2">
+        <v>1</v>
+      </c>
+      <c r="J48" s="2">
+        <v>0</v>
+      </c>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2">
+        <v>2</v>
+      </c>
+      <c r="P48" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2">
+        <v>1</v>
+      </c>
+      <c r="J49" s="2">
+        <v>0</v>
+      </c>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2">
+        <v>2</v>
+      </c>
+      <c r="P49" s="2">
+        <v>2</v>
+      </c>
+      <c r="V49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50" s="2">
+        <v>1</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2">
+        <v>1</v>
+      </c>
+      <c r="J50" s="2">
+        <v>0</v>
+      </c>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2">
+        <v>2</v>
+      </c>
+      <c r="P50" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51" s="2">
+        <v>2</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2">
+        <v>1</v>
+      </c>
+      <c r="J51" s="2">
+        <v>1</v>
+      </c>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2">
+        <v>2</v>
+      </c>
+      <c r="P51" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2">
+        <v>1</v>
+      </c>
+      <c r="J52" s="2">
+        <v>2</v>
+      </c>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2">
+        <v>3</v>
+      </c>
+      <c r="P52" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2">
+        <v>0</v>
+      </c>
+      <c r="J53" s="2">
+        <v>0</v>
+      </c>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2">
+        <v>1</v>
+      </c>
+      <c r="P53" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D54" s="2">
+        <v>2</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2">
+        <v>1</v>
+      </c>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2">
+        <v>0</v>
+      </c>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D56" s="2">
+        <v>2</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2">
+        <v>1</v>
+      </c>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2">
+        <v>0</v>
+      </c>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D58" s="2">
+        <v>2</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2">
+        <v>0</v>
+      </c>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D59" s="2">
+        <v>1</v>
+      </c>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2">
+        <v>0</v>
+      </c>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2">
+        <v>2</v>
+      </c>
+      <c r="V59" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D60" s="2">
+        <v>0</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2">
+        <v>1</v>
+      </c>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D61" s="2">
+        <v>1</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2">
+        <v>0</v>
+      </c>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2">
+        <v>4</v>
+      </c>
+      <c r="V61" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D62" s="2">
+        <v>2</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2">
+        <v>1</v>
+      </c>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
+      <c r="P62" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D63" s="2">
+        <v>1</v>
+      </c>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2">
+        <v>0</v>
+      </c>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
+      <c r="O63" s="2"/>
+      <c r="P63" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2">
+        <v>1</v>
+      </c>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+      <c r="N64" s="2"/>
+      <c r="O64" s="2"/>
+      <c r="P64" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D65" s="2">
+        <v>2</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2">
+        <v>1</v>
+      </c>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
+      <c r="O65" s="2"/>
+      <c r="P65" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2">
+        <v>1</v>
+      </c>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
+      <c r="O66" s="2"/>
+      <c r="P66" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D67" s="2">
+        <v>1</v>
+      </c>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2">
+        <v>0</v>
+      </c>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+      <c r="O67" s="2"/>
+      <c r="P67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D68" s="2">
+        <v>2</v>
+      </c>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2">
+        <v>0</v>
+      </c>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D69" s="2">
+        <v>2</v>
+      </c>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2">
+        <v>1</v>
+      </c>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+      <c r="O69" s="2"/>
+      <c r="P69" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D70" s="2">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2">
+        <v>0</v>
+      </c>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
+      <c r="O70" s="2"/>
+      <c r="P70" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D71" s="2">
+        <v>2</v>
+      </c>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2">
+        <v>1</v>
+      </c>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
+      <c r="N71" s="2"/>
+      <c r="O71" s="2"/>
+      <c r="P71" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D72" s="2">
+        <v>2</v>
+      </c>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2">
+        <v>1</v>
+      </c>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+      <c r="M72" s="2"/>
+      <c r="N72" s="2"/>
+      <c r="O72" s="2"/>
+      <c r="P72" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D73" s="2">
+        <v>2</v>
+      </c>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2">
+        <v>1</v>
+      </c>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+      <c r="N73" s="2"/>
+      <c r="O73" s="2"/>
+      <c r="P73" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D74" s="2">
+        <v>2</v>
+      </c>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2">
+        <v>1</v>
+      </c>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
+      <c r="N74" s="2"/>
+      <c r="O74" s="2"/>
+      <c r="P74" s="2">
+        <v>2</v>
+      </c>
+      <c r="V74" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D75" s="2">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2">
+        <v>1</v>
+      </c>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
+      <c r="O75" s="2"/>
+      <c r="P75" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D76" s="2">
+        <v>2</v>
+      </c>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2">
+        <v>1</v>
+      </c>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
+      <c r="O76" s="2"/>
+      <c r="P76" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D77" s="2">
+        <v>2</v>
+      </c>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2">
+        <v>0</v>
+      </c>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+      <c r="M77" s="2"/>
+      <c r="N77" s="2"/>
+      <c r="O77" s="2"/>
+      <c r="P77" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2">
+        <v>0</v>
+      </c>
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+      <c r="M78" s="2"/>
+      <c r="N78" s="2"/>
+      <c r="O78" s="2"/>
+      <c r="P78" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>99</v>
       </c>
@@ -1385,169 +3048,403 @@
         <v>115</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>2</v>
+      </c>
+      <c r="H104">
+        <v>1</v>
+      </c>
+      <c r="N104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>2</v>
+      </c>
+      <c r="H105">
+        <v>1</v>
+      </c>
+      <c r="N105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>2</v>
+      </c>
+      <c r="H106">
+        <v>1</v>
+      </c>
+      <c r="N106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>2</v>
+      </c>
+      <c r="H107">
+        <v>1</v>
+      </c>
+      <c r="N107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>2</v>
+      </c>
+      <c r="H108">
+        <v>1</v>
+      </c>
+      <c r="N108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>2</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="N109">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>2</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="N110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>2</v>
+      </c>
+      <c r="H111">
+        <v>1</v>
+      </c>
+      <c r="N111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="H112">
+        <v>0</v>
+      </c>
+      <c r="N112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="H113">
+        <v>0</v>
+      </c>
+      <c r="N113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="H114">
+        <v>0</v>
+      </c>
+      <c r="N114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>1</v>
+      </c>
+      <c r="N115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>2</v>
+      </c>
+      <c r="H116">
+        <v>0</v>
+      </c>
+      <c r="N116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>2</v>
+      </c>
+      <c r="H117">
+        <v>1</v>
+      </c>
+      <c r="N117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>2</v>
+      </c>
+      <c r="H118">
+        <v>1</v>
+      </c>
+      <c r="N118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>2</v>
+      </c>
+      <c r="H119">
+        <v>1</v>
+      </c>
+      <c r="N119">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="N120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>1</v>
+      </c>
+      <c r="H121">
+        <v>1</v>
+      </c>
+      <c r="N121">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>0</v>
+      </c>
+      <c r="H122">
+        <v>0</v>
+      </c>
+      <c r="N122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>2</v>
+      </c>
+      <c r="H123">
+        <v>1</v>
+      </c>
+      <c r="N123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>0</v>
+      </c>
+      <c r="H124">
+        <v>1</v>
+      </c>
+      <c r="N124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>2</v>
+      </c>
+      <c r="H125">
+        <v>1</v>
+      </c>
+      <c r="N125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>1</v>
+      </c>
+      <c r="H126">
+        <v>1</v>
+      </c>
+      <c r="N126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="H127">
+        <v>1</v>
+      </c>
+      <c r="N127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>2</v>
+      </c>
+      <c r="H128">
+        <v>1</v>
+      </c>
+      <c r="N128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>148</v>
+      </c>
+      <c r="B129">
+        <v>2</v>
+      </c>
+      <c r="H129">
+        <v>1</v>
+      </c>
+      <c r="N129">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>